<commit_message>
climb rate calculations mathing diagram
</commit_message>
<xml_diff>
--- a/5708745_AE1222II_ACD_2024.xlsx
+++ b/5708745_AE1222II_ACD_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aerospace\ADSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209DF9EA-DF08-475E-94F2-055B5F449DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F38822-57A4-437B-B2CC-317380E16AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{B0EDAE5C-5DAE-4AFD-85A9-74F2333B50BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{B0EDAE5C-5DAE-4AFD-85A9-74F2333B50BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="684">
   <si>
     <t>AE1222-II</t>
   </si>
@@ -3143,15 +3143,6 @@
     <t>Bombardier</t>
   </si>
   <si>
-    <t>24.9</t>
-  </si>
-  <si>
-    <t>71.1</t>
-  </si>
-  <si>
-    <t>8.72</t>
-  </si>
-  <si>
     <t xml:space="preserve">BAe </t>
   </si>
   <si>
@@ -3282,6 +3273,60 @@
   </si>
   <si>
     <t>18.05</t>
+  </si>
+  <si>
+    <t>39.3%</t>
+  </si>
+  <si>
+    <t>0.106</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>68.6</t>
+  </si>
+  <si>
+    <t>23.2</t>
+  </si>
+  <si>
+    <t>7.85</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.566</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>Civilian Jet</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>9.85</t>
   </si>
 </sst>
 </file>
@@ -4413,8 +4458,14 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>1675</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4852,6 +4903,159 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4300</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4909,6 +5113,159 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5119,126 +5476,6 @@
                 <c:pt idx="50">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5248,6 +5485,123 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="91"/>
+                <c:pt idx="12">
+                  <c:v>1.0202067654452471</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.94644742426159068</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8835756194187866</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.82941384364866411</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.78232896650009565</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.74107212351045371</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70467197565325079</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67236167632862809</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.64352774825669845</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.61767356697279163</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.59439280336944966</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5733497942709469</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.55426482036417857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.53690291742613627</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.52106526957581323</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.50658251513679631</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.49330948695787408</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48112104094317465</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.46990871887627578</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.45957805714932576</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.45004640010545444</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.441241110955291</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.43309809841409641</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.42556059591538781</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.4185781442889579</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.41210573941002732</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.40610311443010938</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.40053413243389535</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.39536627019760751</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.39057017749490969</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.38611929935911699</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.38198955105300336</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.37815903736090889</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.37460780930856574</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.37131765261512045</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.36827190315128178</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.36545528546519923</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.36285377108068362</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.36045445379964097</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5443,126 +5797,6 @@
                 <c:pt idx="50">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5572,6 +5806,153 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="91"/>
+                <c:pt idx="2">
+                  <c:v>0.82130749650016799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71890112033637821</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65785477560116268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61619471313205509</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58544253257900647</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56154195175876576</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54227624825008391</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52631818373410844</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51281813557352274</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.50120364805007234</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.49107306016818908</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.48213511995835856</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47417279739589963</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.46702061188719318</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.46054988780058137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.45465885714175019</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44926583216672267</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.44430438252407684</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.43971985656602758</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.43546682539636822</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.43150717367818914</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.42780865228134035</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.42434376628950321</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.42108891024046508</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.41802368815729218</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.41513037344545933</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.41239347587938291</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.40979939145645689</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.40733611700587236</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.40499301585912939</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.40276062412504199</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.40063048950770863</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.39859503639800459</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.39664745232271514</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.39478159186705419</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.39299189497925086</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.39127331718022385</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.38962126968090782</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.3880315677867614</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.38650038626730454</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.38502422060609748</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.38359985323689455</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.38222432402503614</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.38089490437735168</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.37960907446496084</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.37836450312609932</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.37715903008409452</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.37599065017176075</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.37485749930003359</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5766,126 +6147,6 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6090,126 +6351,6 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6437,126 +6578,6 @@
                 <c:pt idx="50">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6768,126 +6789,6 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7103,126 +7004,6 @@
                 <c:pt idx="50">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7434,126 +7215,6 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6700</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6800</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7300</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7400</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7600</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8300</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8600</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8700</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8900</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10657,7 +10318,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -14223,8 +13884,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A23" zoomScale="145" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14452,7 +14113,7 @@
         <v>223</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>45</v>
@@ -15072,8 +14733,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15332,12 +14993,14 @@
         <v>620</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="M8" s="1">
         <v>400</v>
       </c>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>668</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="2"/>
@@ -15351,10 +15014,10 @@
         <v>621</v>
       </c>
       <c r="C9" s="136" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D9" s="1">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1">
         <v>10247</v>
@@ -15363,27 +15026,29 @@
         <v>2876</v>
       </c>
       <c r="G9" s="1">
-        <v>38329</v>
+        <v>33000</v>
       </c>
       <c r="H9" s="1">
-        <v>21845</v>
+        <v>19730</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>623</v>
+        <v>669</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>622</v>
+        <v>670</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>624</v>
+        <v>671</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="M9" s="1">
         <v>389</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="2"/>
@@ -15394,10 +15059,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D10" s="1">
         <v>70</v>
@@ -15415,10 +15080,10 @@
         <v>23300</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="K10" s="1">
         <v>8.98</v>
@@ -15429,7 +15094,9 @@
       <c r="M10" s="1">
         <v>425</v>
       </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>673</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="2"/>
@@ -15440,10 +15107,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D11" s="1">
         <v>72</v>
@@ -15464,18 +15131,20 @@
         <v>61</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="K11" s="1">
         <v>12</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="M11" s="1">
         <v>397</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="2"/>
@@ -15486,7 +15155,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C12" s="1">
         <v>2000</v>
@@ -15507,21 +15176,23 @@
         <v>14500</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="M12" s="1">
         <v>362</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>675</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="2"/>
@@ -15773,7 +15444,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26:G26"/>
     </sheetView>
   </sheetViews>
@@ -15843,7 +15514,7 @@
         <v>98</v>
       </c>
       <c r="B5" s="103" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C5" s="103"/>
       <c r="D5" s="103"/>
@@ -15950,7 +15621,7 @@
         <v>98</v>
       </c>
       <c r="B12" s="103" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C12" s="103"/>
       <c r="D12" s="103"/>
@@ -15982,7 +15653,7 @@
         <v>98</v>
       </c>
       <c r="B14" s="103" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103"/>
@@ -15998,7 +15669,7 @@
         <v>138</v>
       </c>
       <c r="B15" s="103" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C15" s="103"/>
       <c r="D15" s="103"/>
@@ -16014,7 +15685,7 @@
         <v>503</v>
       </c>
       <c r="B16" s="103" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C16" s="103"/>
       <c r="D16" s="103"/>
@@ -16090,7 +15761,7 @@
         <v>118</v>
       </c>
       <c r="B21" s="103" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C21" s="103"/>
       <c r="D21" s="103"/>
@@ -16106,7 +15777,7 @@
         <v>502</v>
       </c>
       <c r="B22" s="103" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C22" s="103"/>
       <c r="D22" s="103"/>
@@ -16150,7 +15821,7 @@
         <v>98</v>
       </c>
       <c r="B25" s="103" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C25" s="103"/>
       <c r="D25" s="103"/>
@@ -16166,7 +15837,7 @@
         <v>501</v>
       </c>
       <c r="B26" s="103" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C26" s="103"/>
       <c r="D26" s="103"/>
@@ -16291,7 +15962,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -16562,7 +16233,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>423</v>
@@ -16630,7 +16301,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>22</v>
@@ -16648,7 +16319,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>22</v>
@@ -16666,7 +16337,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="26" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>22</v>
@@ -16703,7 +16374,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="92" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>22</v>
@@ -16721,7 +16392,7 @@
       <c r="C25" s="105"/>
       <c r="D25" s="108"/>
       <c r="E25" s="104" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F25" s="104"/>
       <c r="G25" s="104"/>
@@ -16737,7 +16408,7 @@
       <c r="C26" s="105"/>
       <c r="D26" s="108"/>
       <c r="E26" s="104" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="F26" s="104"/>
       <c r="G26" s="104"/>
@@ -16953,7 +16624,7 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>24</v>
@@ -16971,7 +16642,7 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="16" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>24</v>
@@ -16989,7 +16660,7 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>24</v>
@@ -17593,8 +17264,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17665,7 +17336,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
@@ -17690,7 +17361,7 @@
       </c>
       <c r="B8" s="108"/>
       <c r="C8" s="104" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D8" s="104"/>
       <c r="E8" s="104"/>
@@ -17703,7 +17374,7 @@
       </c>
       <c r="B9" s="108"/>
       <c r="C9" s="104" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D9" s="104"/>
       <c r="E9" s="104"/>
@@ -17716,7 +17387,7 @@
       </c>
       <c r="B10" s="108"/>
       <c r="C10" s="104" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D10" s="104"/>
       <c r="E10" s="104"/>
@@ -17729,7 +17400,7 @@
       </c>
       <c r="B11" s="108"/>
       <c r="C11" s="104" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D11" s="104"/>
       <c r="E11" s="104"/>
@@ -17787,7 +17458,7 @@
       <c r="B16" s="105"/>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>20</v>
@@ -17828,7 +17499,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>20</v>
@@ -17843,7 +17514,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>20</v>
@@ -17878,7 +17549,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>20</v>
@@ -17893,7 +17564,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>20</v>
@@ -17908,7 +17579,7 @@
       <c r="B25" s="105"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>20</v>
@@ -17923,7 +17594,7 @@
       <c r="B26" s="105"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>20</v>
@@ -18000,8 +17671,8 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="138">
-        <v>0.38</v>
+      <c r="D32" s="138" t="s">
+        <v>666</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>20</v>
@@ -18035,7 +17706,9 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>479</v>
       </c>
@@ -18190,8 +17863,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18292,7 +17965,9 @@
       <c r="A5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>667</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
@@ -18446,7 +18121,9 @@
       <c r="A12" s="31" t="s">
         <v>442</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>676</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
@@ -18512,7 +18189,9 @@
       <c r="A15" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <v>29630</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
@@ -18536,7 +18215,9 @@
       <c r="A16" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>18370</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
@@ -18560,7 +18241,9 @@
       <c r="A17" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>3140</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
@@ -18584,7 +18267,9 @@
       <c r="A18" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>667</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -18757,7 +18442,9 @@
       <c r="A25" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>1675</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>44</v>
       </c>
@@ -18781,7 +18468,9 @@
       <c r="A26" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>3520</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>44</v>
       </c>
@@ -18897,8 +18586,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:CA191"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="E98" zoomScale="65" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19294,7 +18983,9 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
@@ -19330,7 +19021,9 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>682</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
@@ -19366,7 +19059,9 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
@@ -19402,7 +19097,9 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>20</v>
       </c>
@@ -19438,7 +19135,9 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>680</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>20</v>
       </c>
@@ -19474,7 +19173,9 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>681</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
@@ -19612,7 +19313,9 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>65</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>46</v>
       </c>
@@ -19648,7 +19351,9 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
@@ -19684,7 +19389,9 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>683</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>45</v>
       </c>
@@ -19720,7 +19427,9 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>612</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>20</v>
       </c>
@@ -19926,7 +19635,9 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <v>1676</v>
+      </c>
       <c r="E30" s="2" t="s">
         <v>24</v>
       </c>
@@ -19962,7 +19673,9 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>24</v>
       </c>
@@ -19998,7 +19711,9 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>683</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>45</v>
       </c>
@@ -20034,7 +19749,9 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>612</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>20</v>
       </c>
@@ -20070,7 +19787,9 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="1"/>
+      <c r="D34" s="96">
+        <v>1225</v>
+      </c>
       <c r="E34" s="2" t="s">
         <v>423</v>
       </c>
@@ -20242,7 +19961,9 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1">
+        <v>9300</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>24</v>
       </c>
@@ -20312,7 +20033,9 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1">
+        <v>10</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>20</v>
       </c>
@@ -20384,7 +20107,9 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1">
+        <v>212</v>
+      </c>
       <c r="E43" s="2" t="s">
         <v>46</v>
       </c>
@@ -20522,7 +20247,9 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1">
+        <v>3.8</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>46</v>
       </c>
@@ -20558,7 +20285,9 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1">
+        <v>7400</v>
+      </c>
       <c r="E48" s="2" t="s">
         <v>46</v>
       </c>
@@ -20594,7 +20323,9 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1">
+        <v>0.95</v>
+      </c>
       <c r="E49" s="2" t="s">
         <v>20</v>
       </c>
@@ -20630,7 +20361,9 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1">
+        <v>48.1</v>
+      </c>
       <c r="E50" s="2" t="s">
         <v>45</v>
       </c>
@@ -20700,7 +20433,9 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1">
+        <v>240.05</v>
+      </c>
       <c r="E52" s="2" t="s">
         <v>45</v>
       </c>
@@ -20736,7 +20471,9 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1">
+        <v>38800</v>
+      </c>
       <c r="E53" s="2" t="s">
         <v>481</v>
       </c>
@@ -20772,7 +20509,9 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="1"/>
+      <c r="D54" s="1">
+        <v>0.56308000000000002</v>
+      </c>
       <c r="E54" s="2" t="s">
         <v>423</v>
       </c>
@@ -22528,10 +22267,14 @@
       <c r="B100" s="15">
         <v>0</v>
       </c>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
+      <c r="C100" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D100" s="15">
+        <v>4100</v>
+      </c>
       <c r="E100" s="15"/>
-      <c r="F100" s="15"/>
+      <c r="F100" s="16"/>
       <c r="G100" s="15"/>
       <c r="H100" s="15"/>
       <c r="I100" s="15"/>
@@ -22562,10 +22305,14 @@
       <c r="B101" s="15">
         <v>100</v>
       </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
+      <c r="C101" s="16">
+        <v>4300</v>
+      </c>
+      <c r="D101" s="16">
+        <v>4100</v>
+      </c>
       <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
+      <c r="F101" s="16"/>
       <c r="G101" s="15"/>
       <c r="H101" s="15"/>
       <c r="I101" s="15"/>
@@ -22596,10 +22343,17 @@
       <c r="B102" s="15">
         <v>200</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
+      <c r="C102" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D102" s="15">
+        <v>4100</v>
+      </c>
       <c r="E102" s="15"/>
-      <c r="F102" s="15"/>
+      <c r="F102" s="15">
+        <f>4.75*(SQRT(2.6226/(0.95*B102))+0.05542)</f>
+        <v>0.82130749650016799</v>
+      </c>
       <c r="G102" s="15"/>
       <c r="H102" s="15"/>
       <c r="I102" s="15"/>
@@ -22630,10 +22384,17 @@
       <c r="B103" s="15">
         <v>300</v>
       </c>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
+      <c r="C103" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D103" s="15">
+        <v>4100</v>
+      </c>
       <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
+      <c r="F103" s="15">
+        <f t="shared" ref="F103:F150" si="0">4.75*(SQRT(2.6226/(0.95*B103))+0.05542)</f>
+        <v>0.71890112033637821</v>
+      </c>
       <c r="G103" s="15"/>
       <c r="H103" s="15"/>
       <c r="I103" s="15"/>
@@ -22664,10 +22425,17 @@
       <c r="B104" s="15">
         <v>400</v>
       </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
+      <c r="C104" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D104" s="15">
+        <v>4100</v>
+      </c>
       <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
+      <c r="F104" s="15">
+        <f t="shared" si="0"/>
+        <v>0.65785477560116268</v>
+      </c>
       <c r="G104" s="15"/>
       <c r="H104" s="15"/>
       <c r="I104" s="15"/>
@@ -22698,10 +22466,17 @@
       <c r="B105" s="15">
         <v>500</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
+      <c r="C105" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D105" s="15">
+        <v>4100</v>
+      </c>
       <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
+      <c r="F105" s="15">
+        <f t="shared" si="0"/>
+        <v>0.61619471313205509</v>
+      </c>
       <c r="G105" s="15"/>
       <c r="H105" s="15"/>
       <c r="I105" s="15"/>
@@ -22732,10 +22507,17 @@
       <c r="B106" s="15">
         <v>600</v>
       </c>
-      <c r="C106" s="15"/>
-      <c r="D106" s="15"/>
+      <c r="C106" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D106" s="15">
+        <v>4100</v>
+      </c>
       <c r="E106" s="15"/>
-      <c r="F106" s="15"/>
+      <c r="F106" s="15">
+        <f t="shared" si="0"/>
+        <v>0.58544253257900647</v>
+      </c>
       <c r="G106" s="15"/>
       <c r="H106" s="15"/>
       <c r="I106" s="15"/>
@@ -22766,10 +22548,17 @@
       <c r="B107" s="15">
         <v>700</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
+      <c r="C107" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D107" s="15">
+        <v>4100</v>
+      </c>
       <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
+      <c r="F107" s="15">
+        <f t="shared" si="0"/>
+        <v>0.56154195175876576</v>
+      </c>
       <c r="G107" s="15"/>
       <c r="H107" s="15"/>
       <c r="I107" s="15"/>
@@ -22800,10 +22589,17 @@
       <c r="B108" s="15">
         <v>800</v>
       </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
+      <c r="C108" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D108" s="15">
+        <v>4100</v>
+      </c>
       <c r="E108" s="15"/>
-      <c r="F108" s="15"/>
+      <c r="F108" s="15">
+        <f t="shared" si="0"/>
+        <v>0.54227624825008391</v>
+      </c>
       <c r="G108" s="15"/>
       <c r="H108" s="15"/>
       <c r="I108" s="15"/>
@@ -22834,10 +22630,17 @@
       <c r="B109" s="15">
         <v>900</v>
       </c>
-      <c r="C109" s="15"/>
-      <c r="D109" s="15"/>
+      <c r="C109" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D109" s="15">
+        <v>4100</v>
+      </c>
       <c r="E109" s="15"/>
-      <c r="F109" s="15"/>
+      <c r="F109" s="15">
+        <f t="shared" si="0"/>
+        <v>0.52631818373410844</v>
+      </c>
       <c r="G109" s="15"/>
       <c r="H109" s="15"/>
       <c r="I109" s="15"/>
@@ -22868,10 +22671,17 @@
       <c r="B110" s="15">
         <v>1000</v>
       </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15"/>
+      <c r="C110" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D110" s="15">
+        <v>4100</v>
+      </c>
       <c r="E110" s="15"/>
-      <c r="F110" s="15"/>
+      <c r="F110" s="15">
+        <f t="shared" si="0"/>
+        <v>0.51281813557352274</v>
+      </c>
       <c r="G110" s="15"/>
       <c r="H110" s="15"/>
       <c r="I110" s="15"/>
@@ -22902,10 +22712,17 @@
       <c r="B111" s="15">
         <v>1100</v>
       </c>
-      <c r="C111" s="15"/>
-      <c r="D111" s="15"/>
+      <c r="C111" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D111" s="15">
+        <v>4100</v>
+      </c>
       <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
+      <c r="F111" s="15">
+        <f t="shared" si="0"/>
+        <v>0.50120364805007234</v>
+      </c>
       <c r="G111" s="15"/>
       <c r="H111" s="15"/>
       <c r="I111" s="15"/>
@@ -22936,10 +22753,20 @@
       <c r="B112" s="15">
         <v>1200</v>
       </c>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="15"/>
+      <c r="C112" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D112" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E112" s="15">
+        <f t="shared" ref="E102:E165" si="1">6.26*(180.427/(0.95*B112)+(0.95*B112)/242397)</f>
+        <v>1.0202067654452471</v>
+      </c>
+      <c r="F112" s="15">
+        <f t="shared" si="0"/>
+        <v>0.49107306016818908</v>
+      </c>
       <c r="G112" s="15"/>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
@@ -22970,10 +22797,20 @@
       <c r="B113" s="15">
         <v>1300</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15"/>
-      <c r="E113" s="15"/>
-      <c r="F113" s="15"/>
+      <c r="C113" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D113" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E113" s="15">
+        <f t="shared" si="1"/>
+        <v>0.94644742426159068</v>
+      </c>
+      <c r="F113" s="15">
+        <f t="shared" si="0"/>
+        <v>0.48213511995835856</v>
+      </c>
       <c r="G113" s="15"/>
       <c r="H113" s="15"/>
       <c r="I113" s="15"/>
@@ -23004,10 +22841,20 @@
       <c r="B114" s="15">
         <v>1400</v>
       </c>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="15"/>
-      <c r="F114" s="15"/>
+      <c r="C114" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D114" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E114" s="15">
+        <f t="shared" si="1"/>
+        <v>0.8835756194187866</v>
+      </c>
+      <c r="F114" s="15">
+        <f t="shared" si="0"/>
+        <v>0.47417279739589963</v>
+      </c>
       <c r="G114" s="15"/>
       <c r="H114" s="15"/>
       <c r="I114" s="15"/>
@@ -23038,10 +22885,20 @@
       <c r="B115" s="15">
         <v>1500</v>
       </c>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
-      <c r="F115" s="15"/>
+      <c r="C115" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D115" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E115" s="15">
+        <f t="shared" si="1"/>
+        <v>0.82941384364866411</v>
+      </c>
+      <c r="F115" s="15">
+        <f t="shared" si="0"/>
+        <v>0.46702061188719318</v>
+      </c>
       <c r="G115" s="15"/>
       <c r="H115" s="15"/>
       <c r="I115" s="15"/>
@@ -23072,10 +22929,20 @@
       <c r="B116" s="15">
         <v>1600</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
+      <c r="C116" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D116" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E116" s="15">
+        <f t="shared" si="1"/>
+        <v>0.78232896650009565</v>
+      </c>
+      <c r="F116" s="15">
+        <f t="shared" si="0"/>
+        <v>0.46054988780058137</v>
+      </c>
       <c r="G116" s="15"/>
       <c r="H116" s="15"/>
       <c r="I116" s="15"/>
@@ -23106,10 +22973,20 @@
       <c r="B117" s="15">
         <v>1700</v>
       </c>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="15"/>
-      <c r="F117" s="15"/>
+      <c r="C117" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D117" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E117" s="15">
+        <f t="shared" si="1"/>
+        <v>0.74107212351045371</v>
+      </c>
+      <c r="F117" s="15">
+        <f t="shared" si="0"/>
+        <v>0.45465885714175019</v>
+      </c>
       <c r="G117" s="15"/>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
@@ -23140,10 +23017,20 @@
       <c r="B118" s="15">
         <v>1800</v>
       </c>
-      <c r="C118" s="15"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="15"/>
-      <c r="F118" s="15"/>
+      <c r="C118" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D118" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E118" s="15">
+        <f t="shared" si="1"/>
+        <v>0.70467197565325079</v>
+      </c>
+      <c r="F118" s="15">
+        <f t="shared" si="0"/>
+        <v>0.44926583216672267</v>
+      </c>
       <c r="G118" s="15"/>
       <c r="H118" s="15"/>
       <c r="I118" s="15"/>
@@ -23174,10 +23061,20 @@
       <c r="B119" s="15">
         <v>1900</v>
       </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="15"/>
-      <c r="E119" s="15"/>
-      <c r="F119" s="15"/>
+      <c r="C119" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D119" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E119" s="15">
+        <f t="shared" si="1"/>
+        <v>0.67236167632862809</v>
+      </c>
+      <c r="F119" s="15">
+        <f t="shared" si="0"/>
+        <v>0.44430438252407684</v>
+      </c>
       <c r="G119" s="15"/>
       <c r="H119" s="15"/>
       <c r="I119" s="15"/>
@@ -23208,10 +23105,20 @@
       <c r="B120" s="15">
         <v>2000</v>
       </c>
-      <c r="C120" s="15"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="15"/>
-      <c r="F120" s="15"/>
+      <c r="C120" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D120" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E120" s="15">
+        <f t="shared" si="1"/>
+        <v>0.64352774825669845</v>
+      </c>
+      <c r="F120" s="15">
+        <f t="shared" si="0"/>
+        <v>0.43971985656602758</v>
+      </c>
       <c r="G120" s="15"/>
       <c r="H120" s="15"/>
       <c r="I120" s="15"/>
@@ -23242,10 +23149,20 @@
       <c r="B121" s="15">
         <v>2100</v>
       </c>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="15"/>
-      <c r="F121" s="15"/>
+      <c r="C121" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D121" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E121" s="15">
+        <f t="shared" si="1"/>
+        <v>0.61767356697279163</v>
+      </c>
+      <c r="F121" s="15">
+        <f t="shared" si="0"/>
+        <v>0.43546682539636822</v>
+      </c>
       <c r="G121" s="15"/>
       <c r="H121" s="15"/>
       <c r="I121" s="15"/>
@@ -23276,10 +23193,20 @@
       <c r="B122" s="15">
         <v>2200</v>
       </c>
-      <c r="C122" s="15"/>
-      <c r="D122" s="15"/>
-      <c r="E122" s="15"/>
-      <c r="F122" s="15"/>
+      <c r="C122" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D122" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E122" s="15">
+        <f t="shared" si="1"/>
+        <v>0.59439280336944966</v>
+      </c>
+      <c r="F122" s="15">
+        <f t="shared" si="0"/>
+        <v>0.43150717367818914</v>
+      </c>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
@@ -23310,10 +23237,20 @@
       <c r="B123" s="15">
         <v>2300</v>
       </c>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15"/>
-      <c r="E123" s="15"/>
-      <c r="F123" s="15"/>
+      <c r="C123" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D123" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E123" s="15">
+        <f t="shared" si="1"/>
+        <v>0.5733497942709469</v>
+      </c>
+      <c r="F123" s="15">
+        <f t="shared" si="0"/>
+        <v>0.42780865228134035</v>
+      </c>
       <c r="G123" s="15"/>
       <c r="H123" s="15"/>
       <c r="I123" s="15"/>
@@ -23344,10 +23281,20 @@
       <c r="B124" s="15">
         <v>2400</v>
       </c>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="15"/>
+      <c r="C124" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D124" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E124" s="15">
+        <f t="shared" si="1"/>
+        <v>0.55426482036417857</v>
+      </c>
+      <c r="F124" s="15">
+        <f t="shared" si="0"/>
+        <v>0.42434376628950321</v>
+      </c>
       <c r="G124" s="15"/>
       <c r="H124" s="15"/>
       <c r="I124" s="15"/>
@@ -23378,10 +23325,20 @@
       <c r="B125" s="15">
         <v>2500</v>
       </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
+      <c r="C125" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D125" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E125" s="15">
+        <f t="shared" si="1"/>
+        <v>0.53690291742613627</v>
+      </c>
+      <c r="F125" s="15">
+        <f t="shared" si="0"/>
+        <v>0.42108891024046508</v>
+      </c>
       <c r="G125" s="15"/>
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
@@ -23412,10 +23369,20 @@
       <c r="B126" s="15">
         <v>2600</v>
       </c>
-      <c r="C126" s="15"/>
-      <c r="D126" s="15"/>
-      <c r="E126" s="15"/>
-      <c r="F126" s="15"/>
+      <c r="C126" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D126" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E126" s="15">
+        <f t="shared" si="1"/>
+        <v>0.52106526957581323</v>
+      </c>
+      <c r="F126" s="15">
+        <f t="shared" si="0"/>
+        <v>0.41802368815729218</v>
+      </c>
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
       <c r="I126" s="15"/>
@@ -23446,10 +23413,20 @@
       <c r="B127" s="15">
         <v>2700</v>
       </c>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="15"/>
-      <c r="F127" s="15"/>
+      <c r="C127" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D127" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E127" s="15">
+        <f t="shared" si="1"/>
+        <v>0.50658251513679631</v>
+      </c>
+      <c r="F127" s="15">
+        <f t="shared" si="0"/>
+        <v>0.41513037344545933</v>
+      </c>
       <c r="G127" s="15"/>
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
@@ -23480,10 +23457,20 @@
       <c r="B128" s="15">
         <v>2800</v>
       </c>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
-      <c r="E128" s="15"/>
-      <c r="F128" s="15"/>
+      <c r="C128" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D128" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E128" s="15">
+        <f t="shared" si="1"/>
+        <v>0.49330948695787408</v>
+      </c>
+      <c r="F128" s="15">
+        <f t="shared" si="0"/>
+        <v>0.41239347587938291</v>
+      </c>
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
       <c r="I128" s="15"/>
@@ -23514,10 +23501,20 @@
       <c r="B129" s="15">
         <v>2900</v>
       </c>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
-      <c r="F129" s="15"/>
+      <c r="C129" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D129" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E129" s="15">
+        <f t="shared" si="1"/>
+        <v>0.48112104094317465</v>
+      </c>
+      <c r="F129" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40979939145645689</v>
+      </c>
       <c r="G129" s="15"/>
       <c r="H129" s="15"/>
       <c r="I129" s="15"/>
@@ -23548,10 +23545,20 @@
       <c r="B130" s="15">
         <v>3000</v>
       </c>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
-      <c r="E130" s="15"/>
-      <c r="F130" s="15"/>
+      <c r="C130" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D130" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E130" s="15">
+        <f t="shared" si="1"/>
+        <v>0.46990871887627578</v>
+      </c>
+      <c r="F130" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40733611700587236</v>
+      </c>
       <c r="G130" s="15"/>
       <c r="H130" s="15"/>
       <c r="I130" s="15"/>
@@ -23582,10 +23589,20 @@
       <c r="B131" s="15">
         <v>3100</v>
       </c>
-      <c r="C131" s="15"/>
-      <c r="D131" s="15"/>
-      <c r="E131" s="15"/>
-      <c r="F131" s="15"/>
+      <c r="C131" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D131" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E131" s="15">
+        <f t="shared" si="1"/>
+        <v>0.45957805714932576</v>
+      </c>
+      <c r="F131" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40499301585912939</v>
+      </c>
       <c r="G131" s="15"/>
       <c r="H131" s="15"/>
       <c r="I131" s="15"/>
@@ -23616,10 +23633,20 @@
       <c r="B132" s="15">
         <v>3200</v>
       </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="15"/>
-      <c r="F132" s="15"/>
+      <c r="C132" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D132" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E132" s="15">
+        <f t="shared" si="1"/>
+        <v>0.45004640010545444</v>
+      </c>
+      <c r="F132" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40276062412504199</v>
+      </c>
       <c r="G132" s="15"/>
       <c r="H132" s="15"/>
       <c r="I132" s="15"/>
@@ -23650,10 +23677,20 @@
       <c r="B133" s="15">
         <v>3300</v>
       </c>
-      <c r="C133" s="15"/>
-      <c r="D133" s="15"/>
-      <c r="E133" s="15"/>
-      <c r="F133" s="15"/>
+      <c r="C133" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D133" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E133" s="15">
+        <f t="shared" si="1"/>
+        <v>0.441241110955291</v>
+      </c>
+      <c r="F133" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40063048950770863</v>
+      </c>
       <c r="G133" s="15"/>
       <c r="H133" s="15"/>
       <c r="I133" s="15"/>
@@ -23684,10 +23721,20 @@
       <c r="B134" s="15">
         <v>3400</v>
       </c>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
+      <c r="C134" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D134" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E134" s="15">
+        <f t="shared" si="1"/>
+        <v>0.43309809841409641</v>
+      </c>
+      <c r="F134" s="15">
+        <f t="shared" si="0"/>
+        <v>0.39859503639800459</v>
+      </c>
       <c r="G134" s="15"/>
       <c r="H134" s="15"/>
       <c r="I134" s="15"/>
@@ -23718,10 +23765,20 @@
       <c r="B135" s="15">
         <v>3500</v>
       </c>
-      <c r="C135" s="15"/>
-      <c r="D135" s="15"/>
-      <c r="E135" s="15"/>
-      <c r="F135" s="15"/>
+      <c r="C135" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D135" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E135" s="15">
+        <f t="shared" si="1"/>
+        <v>0.42556059591538781</v>
+      </c>
+      <c r="F135" s="15">
+        <f t="shared" si="0"/>
+        <v>0.39664745232271514</v>
+      </c>
       <c r="G135" s="15"/>
       <c r="H135" s="15"/>
       <c r="I135" s="15"/>
@@ -23752,10 +23809,20 @@
       <c r="B136" s="15">
         <v>3600</v>
       </c>
-      <c r="C136" s="15"/>
-      <c r="D136" s="15"/>
-      <c r="E136" s="15"/>
-      <c r="F136" s="15"/>
+      <c r="C136" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D136" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E136" s="15">
+        <f t="shared" si="1"/>
+        <v>0.4185781442889579</v>
+      </c>
+      <c r="F136" s="15">
+        <f t="shared" si="0"/>
+        <v>0.39478159186705419</v>
+      </c>
       <c r="G136" s="15"/>
       <c r="H136" s="15"/>
       <c r="I136" s="15"/>
@@ -23786,10 +23853,20 @@
       <c r="B137" s="15">
         <v>3700</v>
       </c>
-      <c r="C137" s="15"/>
-      <c r="D137" s="15"/>
-      <c r="E137" s="15"/>
-      <c r="F137" s="15"/>
+      <c r="C137" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D137" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E137" s="15">
+        <f t="shared" si="1"/>
+        <v>0.41210573941002732</v>
+      </c>
+      <c r="F137" s="15">
+        <f t="shared" si="0"/>
+        <v>0.39299189497925086</v>
+      </c>
       <c r="G137" s="15"/>
       <c r="H137" s="15"/>
       <c r="I137" s="15"/>
@@ -23820,10 +23897,20 @@
       <c r="B138" s="15">
         <v>3800</v>
       </c>
-      <c r="C138" s="15"/>
-      <c r="D138" s="15"/>
-      <c r="E138" s="15"/>
-      <c r="F138" s="15"/>
+      <c r="C138" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D138" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E138" s="15">
+        <f t="shared" si="1"/>
+        <v>0.40610311443010938</v>
+      </c>
+      <c r="F138" s="15">
+        <f t="shared" si="0"/>
+        <v>0.39127331718022385</v>
+      </c>
       <c r="G138" s="15"/>
       <c r="H138" s="15"/>
       <c r="I138" s="15"/>
@@ -23854,10 +23941,20 @@
       <c r="B139" s="15">
         <v>3900</v>
       </c>
-      <c r="C139" s="15"/>
-      <c r="D139" s="15"/>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
+      <c r="C139" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D139" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E139" s="15">
+        <f t="shared" si="1"/>
+        <v>0.40053413243389535</v>
+      </c>
+      <c r="F139" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38962126968090782</v>
+      </c>
       <c r="G139" s="15"/>
       <c r="H139" s="15"/>
       <c r="I139" s="15"/>
@@ -23888,10 +23985,20 @@
       <c r="B140" s="15">
         <v>4000</v>
       </c>
-      <c r="C140" s="15"/>
-      <c r="D140" s="15"/>
-      <c r="E140" s="15"/>
-      <c r="F140" s="15"/>
+      <c r="C140" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D140" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E140" s="15">
+        <f t="shared" si="1"/>
+        <v>0.39536627019760751</v>
+      </c>
+      <c r="F140" s="15">
+        <f t="shared" si="0"/>
+        <v>0.3880315677867614</v>
+      </c>
       <c r="G140" s="15"/>
       <c r="H140" s="15"/>
       <c r="I140" s="15"/>
@@ -23922,10 +24029,20 @@
       <c r="B141" s="15">
         <v>4100</v>
       </c>
-      <c r="C141" s="15"/>
-      <c r="D141" s="15"/>
-      <c r="E141" s="15"/>
-      <c r="F141" s="15"/>
+      <c r="C141" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D141" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E141" s="15">
+        <f t="shared" si="1"/>
+        <v>0.39057017749490969</v>
+      </c>
+      <c r="F141" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38650038626730454</v>
+      </c>
       <c r="G141" s="15"/>
       <c r="H141" s="15"/>
       <c r="I141" s="15"/>
@@ -23956,10 +24073,20 @@
       <c r="B142" s="15">
         <v>4200</v>
       </c>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-      <c r="E142" s="15"/>
-      <c r="F142" s="15"/>
+      <c r="C142" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D142" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E142" s="15">
+        <f t="shared" si="1"/>
+        <v>0.38611929935911699</v>
+      </c>
+      <c r="F142" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38502422060609748</v>
+      </c>
       <c r="G142" s="15"/>
       <c r="H142" s="15"/>
       <c r="I142" s="15"/>
@@ -23990,10 +24117,20 @@
       <c r="B143" s="15">
         <v>4300</v>
       </c>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
+      <c r="C143" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D143" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E143" s="15">
+        <f t="shared" si="1"/>
+        <v>0.38198955105300336</v>
+      </c>
+      <c r="F143" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38359985323689455</v>
+      </c>
       <c r="G143" s="15"/>
       <c r="H143" s="15"/>
       <c r="I143" s="15"/>
@@ -24024,10 +24161,20 @@
       <c r="B144" s="15">
         <v>4400</v>
       </c>
-      <c r="C144" s="15"/>
-      <c r="D144" s="15"/>
-      <c r="E144" s="15"/>
-      <c r="F144" s="15"/>
+      <c r="C144" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D144" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E144" s="15">
+        <f t="shared" si="1"/>
+        <v>0.37815903736090889</v>
+      </c>
+      <c r="F144" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38222432402503614</v>
+      </c>
       <c r="G144" s="15"/>
       <c r="H144" s="15"/>
       <c r="I144" s="15"/>
@@ -24058,10 +24205,20 @@
       <c r="B145" s="15">
         <v>4500</v>
       </c>
-      <c r="C145" s="15"/>
-      <c r="D145" s="15"/>
-      <c r="E145" s="15"/>
-      <c r="F145" s="15"/>
+      <c r="C145" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D145" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E145" s="15">
+        <f t="shared" si="1"/>
+        <v>0.37460780930856574</v>
+      </c>
+      <c r="F145" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38089490437735168</v>
+      </c>
       <c r="G145" s="15"/>
       <c r="H145" s="15"/>
       <c r="I145" s="15"/>
@@ -24092,10 +24249,20 @@
       <c r="B146" s="15">
         <v>4600</v>
       </c>
-      <c r="C146" s="15"/>
-      <c r="D146" s="15"/>
-      <c r="E146" s="15"/>
-      <c r="F146" s="15"/>
+      <c r="C146" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D146" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E146" s="15">
+        <f t="shared" si="1"/>
+        <v>0.37131765261512045</v>
+      </c>
+      <c r="F146" s="15">
+        <f t="shared" si="0"/>
+        <v>0.37960907446496084</v>
+      </c>
       <c r="G146" s="15"/>
       <c r="H146" s="15"/>
       <c r="I146" s="15"/>
@@ -24126,10 +24293,20 @@
       <c r="B147" s="15">
         <v>4700</v>
       </c>
-      <c r="C147" s="15"/>
-      <c r="D147" s="15"/>
-      <c r="E147" s="15"/>
-      <c r="F147" s="15"/>
+      <c r="C147" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D147" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E147" s="15">
+        <f t="shared" si="1"/>
+        <v>0.36827190315128178</v>
+      </c>
+      <c r="F147" s="15">
+        <f t="shared" si="0"/>
+        <v>0.37836450312609932</v>
+      </c>
       <c r="G147" s="15"/>
       <c r="H147" s="15"/>
       <c r="I147" s="15"/>
@@ -24160,10 +24337,20 @@
       <c r="B148" s="15">
         <v>4800</v>
       </c>
-      <c r="C148" s="15"/>
-      <c r="D148" s="15"/>
-      <c r="E148" s="15"/>
-      <c r="F148" s="15"/>
+      <c r="C148" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D148" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E148" s="15">
+        <f t="shared" si="1"/>
+        <v>0.36545528546519923</v>
+      </c>
+      <c r="F148" s="15">
+        <f t="shared" si="0"/>
+        <v>0.37715903008409452</v>
+      </c>
       <c r="G148" s="15"/>
       <c r="H148" s="15"/>
       <c r="I148" s="15"/>
@@ -24194,10 +24381,20 @@
       <c r="B149" s="15">
         <v>4900</v>
       </c>
-      <c r="C149" s="15"/>
-      <c r="D149" s="15"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="15"/>
+      <c r="C149" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D149" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E149" s="15">
+        <f t="shared" si="1"/>
+        <v>0.36285377108068362</v>
+      </c>
+      <c r="F149" s="15">
+        <f t="shared" si="0"/>
+        <v>0.37599065017176075</v>
+      </c>
       <c r="G149" s="15"/>
       <c r="H149" s="15"/>
       <c r="I149" s="15"/>
@@ -24228,10 +24425,20 @@
       <c r="B150" s="15">
         <v>5000</v>
       </c>
-      <c r="C150" s="15"/>
-      <c r="D150" s="15"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="15"/>
+      <c r="C150" s="15">
+        <v>4300</v>
+      </c>
+      <c r="D150" s="15">
+        <v>4100</v>
+      </c>
+      <c r="E150" s="15">
+        <f t="shared" si="1"/>
+        <v>0.36045445379964097</v>
+      </c>
+      <c r="F150" s="15">
+        <f t="shared" si="0"/>
+        <v>0.37485749930003359</v>
+      </c>
       <c r="G150" s="15"/>
       <c r="H150" s="15"/>
       <c r="I150" s="15"/>
@@ -24259,9 +24466,7 @@
     </row>
     <row r="151" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A151" s="15"/>
-      <c r="B151" s="15">
-        <v>5100</v>
-      </c>
+      <c r="B151" s="15"/>
       <c r="C151" s="15"/>
       <c r="D151" s="15"/>
       <c r="E151" s="15"/>
@@ -24293,9 +24498,7 @@
     </row>
     <row r="152" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A152" s="15"/>
-      <c r="B152" s="15">
-        <v>5200</v>
-      </c>
+      <c r="B152" s="15"/>
       <c r="C152" s="15"/>
       <c r="D152" s="15"/>
       <c r="E152" s="15"/>
@@ -24327,9 +24530,7 @@
     </row>
     <row r="153" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A153" s="15"/>
-      <c r="B153" s="15">
-        <v>5300</v>
-      </c>
+      <c r="B153" s="15"/>
       <c r="C153" s="15"/>
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
@@ -24361,9 +24562,7 @@
     </row>
     <row r="154" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A154" s="15"/>
-      <c r="B154" s="15">
-        <v>5400</v>
-      </c>
+      <c r="B154" s="15"/>
       <c r="C154" s="15"/>
       <c r="D154" s="15"/>
       <c r="E154" s="15"/>
@@ -24395,9 +24594,7 @@
     </row>
     <row r="155" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A155" s="15"/>
-      <c r="B155" s="15">
-        <v>5500</v>
-      </c>
+      <c r="B155" s="15"/>
       <c r="C155" s="15"/>
       <c r="D155" s="15"/>
       <c r="E155" s="15"/>
@@ -24429,9 +24626,7 @@
     </row>
     <row r="156" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A156" s="15"/>
-      <c r="B156" s="15">
-        <v>5600</v>
-      </c>
+      <c r="B156" s="15"/>
       <c r="C156" s="15"/>
       <c r="D156" s="15"/>
       <c r="E156" s="15"/>
@@ -24463,9 +24658,7 @@
     </row>
     <row r="157" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A157" s="15"/>
-      <c r="B157" s="15">
-        <v>5700</v>
-      </c>
+      <c r="B157" s="15"/>
       <c r="C157" s="15"/>
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
@@ -24497,9 +24690,7 @@
     </row>
     <row r="158" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A158" s="15"/>
-      <c r="B158" s="15">
-        <v>5800</v>
-      </c>
+      <c r="B158" s="15"/>
       <c r="C158" s="15"/>
       <c r="D158" s="15"/>
       <c r="E158" s="15"/>
@@ -24531,9 +24722,7 @@
     </row>
     <row r="159" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A159" s="15"/>
-      <c r="B159" s="15">
-        <v>5900</v>
-      </c>
+      <c r="B159" s="15"/>
       <c r="C159" s="15"/>
       <c r="D159" s="15"/>
       <c r="E159" s="15"/>
@@ -24565,9 +24754,7 @@
     </row>
     <row r="160" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A160" s="15"/>
-      <c r="B160" s="15">
-        <v>6000</v>
-      </c>
+      <c r="B160" s="15"/>
       <c r="C160" s="15"/>
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
@@ -24599,9 +24786,7 @@
     </row>
     <row r="161" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A161" s="15"/>
-      <c r="B161" s="15">
-        <v>6100</v>
-      </c>
+      <c r="B161" s="15"/>
       <c r="C161" s="15"/>
       <c r="D161" s="15"/>
       <c r="E161" s="15"/>
@@ -24633,9 +24818,7 @@
     </row>
     <row r="162" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A162" s="15"/>
-      <c r="B162" s="15">
-        <v>6200</v>
-      </c>
+      <c r="B162" s="15"/>
       <c r="C162" s="15"/>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
@@ -24667,9 +24850,7 @@
     </row>
     <row r="163" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A163" s="15"/>
-      <c r="B163" s="15">
-        <v>6300</v>
-      </c>
+      <c r="B163" s="15"/>
       <c r="C163" s="15"/>
       <c r="D163" s="15"/>
       <c r="E163" s="15"/>
@@ -24701,9 +24882,7 @@
     </row>
     <row r="164" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A164" s="15"/>
-      <c r="B164" s="15">
-        <v>6400</v>
-      </c>
+      <c r="B164" s="15"/>
       <c r="C164" s="15"/>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
@@ -24735,9 +24914,7 @@
     </row>
     <row r="165" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A165" s="15"/>
-      <c r="B165" s="15">
-        <v>6500</v>
-      </c>
+      <c r="B165" s="15"/>
       <c r="C165" s="15"/>
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
@@ -24769,9 +24946,7 @@
     </row>
     <row r="166" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A166" s="15"/>
-      <c r="B166" s="15">
-        <v>6600</v>
-      </c>
+      <c r="B166" s="15"/>
       <c r="C166" s="15"/>
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
@@ -24803,9 +24978,7 @@
     </row>
     <row r="167" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A167" s="15"/>
-      <c r="B167" s="15">
-        <v>6700</v>
-      </c>
+      <c r="B167" s="15"/>
       <c r="C167" s="15"/>
       <c r="D167" s="15"/>
       <c r="E167" s="15"/>
@@ -24837,9 +25010,7 @@
     </row>
     <row r="168" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A168" s="15"/>
-      <c r="B168" s="15">
-        <v>6800</v>
-      </c>
+      <c r="B168" s="15"/>
       <c r="C168" s="15"/>
       <c r="D168" s="15"/>
       <c r="E168" s="15"/>
@@ -24871,9 +25042,7 @@
     </row>
     <row r="169" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A169" s="15"/>
-      <c r="B169" s="15">
-        <v>6900</v>
-      </c>
+      <c r="B169" s="15"/>
       <c r="C169" s="15"/>
       <c r="D169" s="15"/>
       <c r="E169" s="15"/>
@@ -24905,9 +25074,7 @@
     </row>
     <row r="170" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A170" s="15"/>
-      <c r="B170" s="15">
-        <v>7000</v>
-      </c>
+      <c r="B170" s="15"/>
       <c r="C170" s="15"/>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
@@ -24939,9 +25106,7 @@
     </row>
     <row r="171" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A171" s="15"/>
-      <c r="B171" s="15">
-        <v>7100</v>
-      </c>
+      <c r="B171" s="15"/>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
       <c r="E171" s="15"/>
@@ -24973,9 +25138,7 @@
     </row>
     <row r="172" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A172" s="15"/>
-      <c r="B172" s="15">
-        <v>7200</v>
-      </c>
+      <c r="B172" s="15"/>
       <c r="C172" s="15"/>
       <c r="D172" s="15"/>
       <c r="E172" s="15"/>
@@ -25007,9 +25170,7 @@
     </row>
     <row r="173" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A173" s="15"/>
-      <c r="B173" s="15">
-        <v>7300</v>
-      </c>
+      <c r="B173" s="15"/>
       <c r="C173" s="15"/>
       <c r="D173" s="15"/>
       <c r="E173" s="15"/>
@@ -25041,9 +25202,7 @@
     </row>
     <row r="174" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A174" s="15"/>
-      <c r="B174" s="15">
-        <v>7400</v>
-      </c>
+      <c r="B174" s="15"/>
       <c r="C174" s="15"/>
       <c r="D174" s="15"/>
       <c r="E174" s="15"/>
@@ -25075,9 +25234,7 @@
     </row>
     <row r="175" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A175" s="15"/>
-      <c r="B175" s="15">
-        <v>7500</v>
-      </c>
+      <c r="B175" s="15"/>
       <c r="C175" s="15"/>
       <c r="D175" s="15"/>
       <c r="E175" s="15"/>
@@ -25109,9 +25266,7 @@
     </row>
     <row r="176" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A176" s="15"/>
-      <c r="B176" s="15">
-        <v>7600</v>
-      </c>
+      <c r="B176" s="15"/>
       <c r="C176" s="15"/>
       <c r="D176" s="15"/>
       <c r="E176" s="15"/>
@@ -25143,9 +25298,7 @@
     </row>
     <row r="177" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A177" s="15"/>
-      <c r="B177" s="15">
-        <v>7700</v>
-      </c>
+      <c r="B177" s="15"/>
       <c r="C177" s="15"/>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
@@ -25177,9 +25330,7 @@
     </row>
     <row r="178" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A178" s="15"/>
-      <c r="B178" s="15">
-        <v>7800</v>
-      </c>
+      <c r="B178" s="15"/>
       <c r="C178" s="15"/>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
@@ -25211,9 +25362,7 @@
     </row>
     <row r="179" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A179" s="15"/>
-      <c r="B179" s="15">
-        <v>7900</v>
-      </c>
+      <c r="B179" s="15"/>
       <c r="C179" s="15"/>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
@@ -25245,9 +25394,7 @@
     </row>
     <row r="180" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A180" s="15"/>
-      <c r="B180" s="15">
-        <v>8000</v>
-      </c>
+      <c r="B180" s="15"/>
       <c r="C180" s="15"/>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
@@ -25279,9 +25426,7 @@
     </row>
     <row r="181" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A181" s="15"/>
-      <c r="B181" s="15">
-        <v>8100</v>
-      </c>
+      <c r="B181" s="15"/>
       <c r="C181" s="15"/>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
@@ -25313,9 +25458,7 @@
     </row>
     <row r="182" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A182" s="15"/>
-      <c r="B182" s="15">
-        <v>8200</v>
-      </c>
+      <c r="B182" s="15"/>
       <c r="C182" s="15"/>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
@@ -25347,9 +25490,7 @@
     </row>
     <row r="183" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A183" s="15"/>
-      <c r="B183" s="15">
-        <v>8300</v>
-      </c>
+      <c r="B183" s="15"/>
       <c r="C183" s="15"/>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
@@ -25381,9 +25522,7 @@
     </row>
     <row r="184" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A184" s="15"/>
-      <c r="B184" s="15">
-        <v>8400</v>
-      </c>
+      <c r="B184" s="15"/>
       <c r="C184" s="15"/>
       <c r="D184" s="15"/>
       <c r="E184" s="15"/>
@@ -25415,9 +25554,7 @@
     </row>
     <row r="185" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A185" s="15"/>
-      <c r="B185" s="15">
-        <v>8500</v>
-      </c>
+      <c r="B185" s="15"/>
       <c r="C185" s="15"/>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
@@ -25449,9 +25586,7 @@
     </row>
     <row r="186" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A186" s="15"/>
-      <c r="B186" s="15">
-        <v>8600</v>
-      </c>
+      <c r="B186" s="15"/>
       <c r="C186" s="15"/>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
@@ -25483,9 +25618,7 @@
     </row>
     <row r="187" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A187" s="15"/>
-      <c r="B187" s="15">
-        <v>8700</v>
-      </c>
+      <c r="B187" s="15"/>
       <c r="C187" s="15"/>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
@@ -25517,9 +25650,7 @@
     </row>
     <row r="188" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A188" s="15"/>
-      <c r="B188" s="15">
-        <v>8800</v>
-      </c>
+      <c r="B188" s="15"/>
       <c r="C188" s="15"/>
       <c r="D188" s="15"/>
       <c r="E188" s="15"/>
@@ -25551,9 +25682,7 @@
     </row>
     <row r="189" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A189" s="15"/>
-      <c r="B189" s="15">
-        <v>8900</v>
-      </c>
+      <c r="B189" s="15"/>
       <c r="C189" s="15"/>
       <c r="D189" s="15"/>
       <c r="E189" s="15"/>
@@ -25585,9 +25714,7 @@
     </row>
     <row r="190" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A190" s="15"/>
-      <c r="B190" s="15">
-        <v>9000</v>
-      </c>
+      <c r="B190" s="15"/>
       <c r="C190" s="15"/>
       <c r="D190" s="15"/>
       <c r="E190" s="15"/>

</xml_diff>